<commit_message>
VRT Project updated to Local git
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/SetupTestData.xlsx
+++ b/src/test/resources/TestData/SetupTestData.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stored-Code\TestAutomation\Development\Root\Source\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E050F87-46A1-4331-B296-39871E191E26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C430BF-0BB1-4223-824A-FA923B11C83F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" activeTab="1" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" activeTab="2" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupCreation" sheetId="19" r:id="rId1"/>
     <sheet name="SetupCreation_1" sheetId="20" r:id="rId2"/>
-    <sheet name="SetupCreation_2" sheetId="17" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="18" r:id="rId4"/>
-    <sheet name="SET003" sheetId="2" r:id="rId5"/>
-    <sheet name="SET004" sheetId="10" r:id="rId6"/>
-    <sheet name="SET005" sheetId="1" r:id="rId7"/>
-    <sheet name="SET008" sheetId="3" r:id="rId8"/>
-    <sheet name="SET009" sheetId="11" r:id="rId9"/>
-    <sheet name="SET010" sheetId="4" r:id="rId10"/>
-    <sheet name="SET015" sheetId="5" r:id="rId11"/>
-    <sheet name="SET016" sheetId="12" r:id="rId12"/>
-    <sheet name="SET017" sheetId="6" r:id="rId13"/>
-    <sheet name="SET018" sheetId="7" r:id="rId14"/>
-    <sheet name="SET019" sheetId="14" r:id="rId15"/>
-    <sheet name="SET020" sheetId="8" r:id="rId16"/>
-    <sheet name="SET021" sheetId="15" r:id="rId17"/>
-    <sheet name="SET022" sheetId="16" r:id="rId18"/>
+    <sheet name="SetupCreation_3" sheetId="21" r:id="rId3"/>
+    <sheet name="SetupCreation_4" sheetId="22" r:id="rId4"/>
+    <sheet name="SetupCreation_2" sheetId="17" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId6"/>
+    <sheet name="SET003" sheetId="2" r:id="rId7"/>
+    <sheet name="SET004" sheetId="10" r:id="rId8"/>
+    <sheet name="SET005" sheetId="1" r:id="rId9"/>
+    <sheet name="SET008" sheetId="3" r:id="rId10"/>
+    <sheet name="SET009" sheetId="11" r:id="rId11"/>
+    <sheet name="SET010" sheetId="4" r:id="rId12"/>
+    <sheet name="SET015" sheetId="5" r:id="rId13"/>
+    <sheet name="SET016" sheetId="12" r:id="rId14"/>
+    <sheet name="SET017" sheetId="6" r:id="rId15"/>
+    <sheet name="SET018" sheetId="7" r:id="rId16"/>
+    <sheet name="SET019" sheetId="14" r:id="rId17"/>
+    <sheet name="SET020" sheetId="8" r:id="rId18"/>
+    <sheet name="SET021" sheetId="15" r:id="rId19"/>
+    <sheet name="SET022" sheetId="16" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SetupCreation!$A$1:$Z$51</definedName>
@@ -131,6 +133,80 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{3F1ADC6C-7FB2-42AE-A250-19108C1DB68E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter the data in Yr:Mnth:Dt:Hr:Mnt:Sec format. Ex:- 0:0:0:1:0:0, which means one want to set TOD by 1 Hr ahead of the current time stamp.
+- Enter numeric data.
+- This field is applicable if Qstart is set to TOD
+- If Qstart = Manual, then simply enter 0:0:0:0:0:0</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{8C488893-8A96-4A12-A298-8D5D08A37B88}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter the data in Yr:Mnth:Dt:Hr:Mnt:Sec format. Ex:- 0:0:0:1:0:0, which means one want to set TOD by 1 Hr ahead of the current time stamp.
+- Enter numeric data.
+- This field is applicable if Qstart is set to TOD
+- If Qstart = Manual, then simply enter 0:0:0:0:0:0</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
     <comment ref="M1" authorId="0" shapeId="0" xr:uid="{9DA06F53-D746-4FD1-9674-27D98D617B5C}">
       <text>
         <r>
@@ -163,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3424" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="755">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -2410,6 +2486,24 @@
   </si>
   <si>
     <t>Re-Read</t>
+  </si>
+  <si>
+    <t>Qual_case_010</t>
+  </si>
+  <si>
+    <t>AST0911</t>
+  </si>
+  <si>
+    <t>0901</t>
+  </si>
+  <si>
+    <t>During Entire Study</t>
+  </si>
+  <si>
+    <t>AST0902</t>
+  </si>
+  <si>
+    <t>0912</t>
   </si>
 </sst>
 </file>
@@ -7006,6 +7100,123 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014BDF4D-CBB5-4F9C-BB9D-27B4EA7688A0}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>301</v>
+      </c>
+      <c r="B7" s="2">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2049F43F-94DE-444E-8AA7-927124D09D45}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3299206D-8880-48B7-8144-E8CD00C5D1F6}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -7256,7 +7467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE30440-E635-4D52-A1CC-D1E4951C2625}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -7291,7 +7502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D38FF2F-E585-4F1A-9A4E-9EDA6AE30354}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -7406,7 +7617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDC6971-A18E-444E-9493-5CE9E01DA64C}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -7679,7 +7890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE32352-9683-412A-B278-9DA687CA0934}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -7714,7 +7925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D38C88-FDD6-49E5-8013-685829D33A51}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -7829,7 +8040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2AD9DE-E990-4788-8991-F092345FE2E6}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -8102,7 +8313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937DD162-7CAA-4645-8222-89BAFB37D394}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -8153,54 +8364,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85968853-1FFA-46D5-9B3F-D01D330E203B}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E6EA59-4485-4F31-B12C-06AF6BC0EF0F}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10079,7 +10248,407 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85968853-1FFA-46D5-9B3F-D01D330E203B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694AE40C-7218-4986-989B-672275CB1F5B}">
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>510</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>753</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>754</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>511</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>611</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>661</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>683</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>705</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>725</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>752</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y2" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z2" s="29" t="s">
+        <v>639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F53CE7-4B94-40F0-B2B0-1EC3D68F29F2}">
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>510</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>750</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>511</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>611</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>749</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>683</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>705</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>725</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y2" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z2" s="29" t="s">
+        <v>639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE62EE4E-9060-4348-B013-B5B88C30F8F1}">
   <dimension ref="A1:U51"/>
   <sheetViews>
@@ -13431,7 +14000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2588EC10-D4E8-4199-9BE4-448B0CA5FBB1}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -13623,7 +14192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAF0D48-3FFE-4E63-90D8-6D4600BE85B6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -13659,7 +14228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E449FC5-5B23-47AB-A657-9AEA716ABD07}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -13750,7 +14319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F772A9F6-A3B5-402F-8C68-9034BA270367}">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -14035,121 +14604,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014BDF4D-CBB5-4F9C-BB9D-27B4EA7688A0}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="2">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>301</v>
-      </c>
-      <c r="B7" s="2">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2049F43F-94DE-444E-8AA7-927124D09D45}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>